<commit_message>
Updates from last meeting
</commit_message>
<xml_diff>
--- a/Subject Topics - Series V - lcsh.xlsx
+++ b/Subject Topics - Series V - lcsh.xlsx
@@ -14,7 +14,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet2!#REF!</definedName>
     <definedName name="_xlnm.Extract" localSheetId="0">Sheet2!$A$1</definedName>
   </definedNames>
-  <calcPr calcId="0"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
@@ -1477,12 +1477,12 @@
   <dimension ref="A1:B347"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="B2" sqref="A2:B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="44.28515625" customWidth="1"/>
+    <col min="1" max="1" width="51.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>